<commit_message>
add pcl_viewer_cmds.txt and *.cam
</commit_message>
<xml_diff>
--- a/data/calibration_parameter.xlsx
+++ b/data/calibration_parameter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\uniform_coordinate\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\data_fuse_demo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BA28B9-24A8-4EBA-ABE5-DC3AE9A1DCE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0D4E28-0FE5-4845-A835-62C2AD1BFDB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,6 +92,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="0.000_ "/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,7 +157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -163,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -449,7 +452,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -495,10 +498,10 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>0.49980154305691199</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <v>0.99999847691328703</v>
       </c>
     </row>
@@ -507,10 +510,10 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>-0.50303161620248704</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <v>0</v>
       </c>
     </row>
@@ -519,10 +522,10 @@
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>0.49977981143868</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <v>0</v>
       </c>
     </row>
@@ -531,10 +534,10 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>-0.49737083824542699</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="5">
         <v>1.7453283658982999E-3</v>
       </c>
     </row>
@@ -545,13 +548,11 @@
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2">
-        <f>1.70079118954*1000</f>
-        <v>1700.79118954</v>
-      </c>
-      <c r="D7" s="2">
-        <f>3.412*1000</f>
-        <v>3412</v>
+      <c r="C7" s="5">
+        <v>1.7007911895400001</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3.4119999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
@@ -559,11 +560,10 @@
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2">
-        <f>0.0159456324149*1000</f>
-        <v>15.9456324149</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="5">
+        <v>1.5945632414900001E-2</v>
+      </c>
+      <c r="D8" s="5">
         <v>0</v>
       </c>
     </row>
@@ -572,50 +572,48 @@
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2">
-        <f>1.51095763913*1000</f>
-        <v>1510.95763913</v>
-      </c>
-      <c r="D9" s="2">
-        <f>0.5*1000</f>
-        <v>500</v>
+      <c r="C9" s="5">
+        <v>1.5109576391299999</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="2">
         <v>1266.41720304655</v>
       </c>
-      <c r="C10" s="5">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
         <v>816.26701974479795</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
         <v>1266.41720304655</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="2">
         <v>491.507065792947</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>